<commit_message>
feat: add works and third course test scripts.
</commit_message>
<xml_diff>
--- a/course/work/第二次作业.xlsx
+++ b/course/work/第二次作业.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\StableDiffusionEO\course\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD68966D-C777-41E8-B73B-C8BBFA977701}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B6B046-0E74-45CF-9181-CAA1925C864A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>clip</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,6 +98,14 @@
   </si>
   <si>
     <t>base（fp16）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>base</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attention work3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -466,7 +474,7 @@
   <dimension ref="A3:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -587,6 +595,19 @@
         <v>1.73041</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>8.74451</v>
+      </c>
+    </row>
     <row r="17" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">

</xml_diff>